<commit_message>
add updated vorarlberg data, adapt make_population to accept school_enrollment_counts_available and use_default
</commit_message>
<xml_diff>
--- a/data/demographics/contact_matrices_152_countries/Austria/VorarlbergHaushalteDaten.xlsx
+++ b/data/demographics/contact_matrices_152_countries/Austria/VorarlbergHaushalteDaten.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Altersgruppen_5Jahre" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,10 +17,10 @@
     <sheet name="ArbeitgebergrößeVerteilung" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="Schulbesuchsquote" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -258,17 +258,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="8">
+  <numFmts count="9">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.0,_)"/>
     <numFmt numFmtId="166" formatCode="\(#,##0.0,\)"/>
     <numFmt numFmtId="167" formatCode="&quot;(x)&quot;"/>
-    <numFmt numFmtId="168" formatCode="0.0_)"/>
-    <numFmt numFmtId="169" formatCode="&quot;household_head_age_&quot;@"/>
-    <numFmt numFmtId="170" formatCode="@"/>
-    <numFmt numFmtId="171" formatCode="#,##0"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00\ _D_M_-;\-* #,##0.00\ _D_M_-;_-* \-??\ _D_M_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="0.0_)"/>
+    <numFmt numFmtId="170" formatCode="&quot;household_head_age_&quot;@"/>
+    <numFmt numFmtId="171" formatCode="@"/>
+    <numFmt numFmtId="172" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -301,6 +302,12 @@
       <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -348,7 +355,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="24">
+  <cellStyleXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -381,8 +388,19 @@
     <xf numFmtId="167" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="12">
@@ -398,11 +416,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -410,32 +428,32 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="172" fontId="4" fillId="0" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="13">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -445,7 +463,10 @@
     <cellStyle name="AZ1" xfId="20"/>
     <cellStyle name="AZ2" xfId="21"/>
     <cellStyle name="AZ3" xfId="22"/>
-    <cellStyle name="PZ1" xfId="23"/>
+    <cellStyle name="Komma 2" xfId="23"/>
+    <cellStyle name="PZ1" xfId="24"/>
+    <cellStyle name="Standard 20" xfId="25"/>
+    <cellStyle name="Standard 6" xfId="26"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -455,15 +476,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,201 +506,182 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.054618593865503</v>
+        <v>0.0564534842660694</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>0.051960446771237</v>
+        <v>0.0540976825368</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>0.053362935809545</v>
+        <v>0.0538353662842903</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>0.054899597986897</v>
+        <v>0.0558683172412402</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>0.059020991767339</v>
+        <v>0.0615989184499127</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>0.065970147742347</v>
+        <v>0.0674859005014276</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>0.068235901694126</v>
+        <v>0.0691960006860579</v>
       </c>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>0.006916245582413</v>
+        <v>0.0702452656960965</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="n">
-        <v>0.065684080483631</v>
+        <v>0.0657253548836224</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2" t="n">
-        <v>0.074058509614898</v>
+        <v>0.0699678158136344</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2" t="n">
-        <v>0.080329205188703</v>
+        <v>0.0797340516763018</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="2" t="n">
-        <v>0.07219274351159</v>
+        <v>0.0767123702291232</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>0.057312182921025</v>
+        <v>0.0606253215896365</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>0.047790953186232</v>
+        <v>0.045532047983696</v>
       </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="2" t="n">
-        <v>0.04060129818841</v>
+        <v>0.0406993754855373</v>
       </c>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="2" t="n">
-        <v>0.038434275414418</v>
+        <v>0.032446502618118</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>0.002369548266888</v>
+        <v>0.0236942199622668</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="2" t="n">
-        <v>0.014931191963789</v>
+        <v>0.0113552670076778</v>
       </c>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>0.006275758711128</v>
+        <v>0.00408608008716971</v>
       </c>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>0.001463246686177</v>
+        <v>0.00064065700132167</v>
       </c>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-    </row>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E1" r:id="rId1" display="https://presse.vorarlberg.at/land/servlet/AttachmentServlet?action=show&amp;id=37826"/>
@@ -705,9 +707,9 @@
       <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>25</v>
@@ -728,7 +730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -751,7 +753,7 @@
         <v>11.6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="n">
         <f aca="false">SUM(C3:G3)</f>
         <v>1</v>
@@ -777,7 +779,7 @@
         <v>0.0687611144042679</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -785,7 +787,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="140.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -793,7 +795,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
@@ -801,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>1</v>
       </c>
@@ -809,7 +811,7 @@
         <v>0.33787788974511</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>2</v>
       </c>
@@ -817,7 +819,7 @@
         <v>0.307053941908714</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>3</v>
       </c>
@@ -825,7 +827,7 @@
         <v>0.150563129816242</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>4</v>
       </c>
@@ -833,7 +835,7 @@
         <v>0.135743924125667</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>5</v>
       </c>
@@ -866,12 +868,12 @@
       <selection pane="topLeft" activeCell="N21" activeCellId="0" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="33.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="33.57"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -912,7 +914,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
@@ -953,7 +955,7 @@
         <v>105049</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
@@ -994,7 +996,7 @@
         <v>111042</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
@@ -1035,7 +1037,7 @@
         <v>16221</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>1547</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
@@ -1117,31 +1119,31 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -1149,7 +1151,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -1157,7 +1159,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
@@ -1187,9 +1189,9 @@
       <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="89.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1209,7 +1211,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1220,7 +1222,7 @@
         <v>0.483615295480881</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -1231,7 +1233,7 @@
         <v>0.488282582216809</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1242,7 +1244,7 @@
         <v>0.489349589638977</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1255,7 @@
         <v>0.480724891635156</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -1264,7 +1266,7 @@
         <v>0.89891874180865</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1275,7 +1277,7 @@
         <v>0.487624237307648</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1286,7 +1288,7 @@
         <v>0.491875046375306</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1297,7 +1299,7 @@
         <v>0.502379209370425</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1308,7 +1310,7 @@
         <v>0.497456255299468</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>0.503042318999111</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>0.488544325738237</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
@@ -1341,7 +1343,7 @@
         <v>0.499421397762738</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1352,7 +1354,7 @@
         <v>0.0941810168938219</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1363,7 +1365,7 @@
         <v>0.52373132747113</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
@@ -1374,7 +1376,7 @@
         <v>0.531051253273475</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
@@ -1385,7 +1387,7 @@
         <v>0.54380187063628</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>0.589209401709402</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1407,7 +1409,7 @@
         <v>0.633604611732791</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
@@ -1418,7 +1420,7 @@
         <v>0.711577248890682</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
@@ -1450,13 +1452,13 @@
   </sheetPr>
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A67" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D84" activeCellId="0" sqref="D84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -1473,7 +1475,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>15</v>
       </c>
@@ -1487,7 +1489,7 @@
         <v>0.441</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>16</v>
       </c>
@@ -1501,7 +1503,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>17</v>
       </c>
@@ -1515,7 +1517,7 @@
         <v>0.842</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>18</v>
       </c>
@@ -1529,7 +1531,7 @@
         <v>0.847</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>19</v>
       </c>
@@ -1543,7 +1545,7 @@
         <v>0.839</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>20</v>
       </c>
@@ -1557,7 +1559,7 @@
         <v>0.835</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>21</v>
       </c>
@@ -1571,7 +1573,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>22</v>
       </c>
@@ -1585,7 +1587,7 @@
         <v>0.738</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>23</v>
       </c>
@@ -1600,7 +1602,7 @@
       </c>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>24</v>
       </c>
@@ -1614,7 +1616,7 @@
         <v>0.119</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>25</v>
       </c>
@@ -1625,7 +1627,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>26</v>
       </c>
@@ -1634,7 +1636,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>27</v>
       </c>
@@ -1642,7 +1644,7 @@
         <v>0.842</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>28</v>
       </c>
@@ -1651,7 +1653,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>29</v>
       </c>
@@ -1660,7 +1662,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>30</v>
       </c>
@@ -1668,7 +1670,7 @@
         <v>0.847</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>31</v>
       </c>
@@ -1677,7 +1679,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>32</v>
       </c>
@@ -1686,7 +1688,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>33</v>
       </c>
@@ -1694,7 +1696,7 @@
         <v>0.847</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>34</v>
       </c>
@@ -1703,7 +1705,7 @@
       </c>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>35</v>
       </c>
@@ -1712,7 +1714,7 @@
       </c>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>36</v>
       </c>
@@ -1720,7 +1722,7 @@
         <v>0.839</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>37</v>
       </c>
@@ -1729,7 +1731,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>38</v>
       </c>
@@ -1738,7 +1740,7 @@
       </c>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>39</v>
       </c>
@@ -1746,7 +1748,7 @@
         <v>0.839</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>40</v>
       </c>
@@ -1755,7 +1757,7 @@
       </c>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>41</v>
       </c>
@@ -1764,7 +1766,7 @@
       </c>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>42</v>
       </c>
@@ -1772,7 +1774,7 @@
         <v>0.835</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>43</v>
       </c>
@@ -1781,7 +1783,7 @@
       </c>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>44</v>
       </c>
@@ -1790,7 +1792,7 @@
       </c>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>45</v>
       </c>
@@ -1798,7 +1800,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>46</v>
       </c>
@@ -1807,7 +1809,7 @@
       </c>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>47</v>
       </c>
@@ -1816,7 +1818,7 @@
       </c>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>48</v>
       </c>
@@ -1824,7 +1826,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>49</v>
       </c>
@@ -1833,7 +1835,7 @@
       </c>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>50</v>
       </c>
@@ -1842,7 +1844,7 @@
       </c>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <v>51</v>
       </c>
@@ -1850,7 +1852,7 @@
         <v>0.738</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>52</v>
       </c>
@@ -1859,7 +1861,7 @@
       </c>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>53</v>
       </c>
@@ -1868,7 +1870,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>54</v>
       </c>
@@ -1876,7 +1878,7 @@
         <v>0.738</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
         <v>55</v>
       </c>
@@ -1885,7 +1887,7 @@
       </c>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
         <v>56</v>
       </c>
@@ -1894,7 +1896,7 @@
       </c>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
         <v>57</v>
       </c>
@@ -1902,7 +1904,7 @@
         <v>0.465</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
         <v>58</v>
       </c>
@@ -1911,7 +1913,7 @@
       </c>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
         <v>59</v>
       </c>
@@ -1920,7 +1922,7 @@
       </c>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
         <v>60</v>
       </c>
@@ -1928,7 +1930,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
         <v>61</v>
       </c>
@@ -1937,7 +1939,7 @@
       </c>
       <c r="D48" s="2"/>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
         <v>62</v>
       </c>
@@ -1946,7 +1948,7 @@
       </c>
       <c r="D49" s="2"/>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
         <v>63</v>
       </c>
@@ -1954,7 +1956,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <v>64</v>
       </c>
@@ -1963,7 +1965,7 @@
       </c>
       <c r="D51" s="2"/>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
         <v>65</v>
       </c>
@@ -1972,7 +1974,7 @@
       </c>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
         <v>66</v>
       </c>
@@ -1980,7 +1982,7 @@
         <v>0.119</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
         <v>67</v>
       </c>
@@ -1988,7 +1990,7 @@
         <v>0.119</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
         <v>68</v>
       </c>
@@ -1996,7 +1998,7 @@
         <v>0.119</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
         <v>69</v>
       </c>
@@ -2004,7 +2006,7 @@
         <v>0.119</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
         <v>70</v>
       </c>
@@ -2012,7 +2014,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
         <v>71</v>
       </c>
@@ -2020,7 +2022,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
         <v>72</v>
       </c>
@@ -2028,7 +2030,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
         <v>73</v>
       </c>
@@ -2036,7 +2038,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
         <v>74</v>
       </c>
@@ -2044,7 +2046,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
         <v>75</v>
       </c>
@@ -2052,7 +2054,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
         <v>76</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
         <v>77</v>
       </c>
@@ -2068,7 +2070,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
         <v>78</v>
       </c>
@@ -2076,7 +2078,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
         <v>79</v>
       </c>
@@ -2084,7 +2086,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
         <v>80</v>
       </c>
@@ -2092,7 +2094,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
         <v>81</v>
       </c>
@@ -2100,7 +2102,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
         <v>82</v>
       </c>
@@ -2108,7 +2110,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
         <v>83</v>
       </c>
@@ -2116,7 +2118,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
         <v>84</v>
       </c>
@@ -2124,7 +2126,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
         <v>85</v>
       </c>
@@ -2132,7 +2134,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
         <v>86</v>
       </c>
@@ -2140,7 +2142,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
         <v>87</v>
       </c>
@@ -2148,7 +2150,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
         <v>88</v>
       </c>
@@ -2156,7 +2158,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
         <v>89</v>
       </c>
@@ -2164,7 +2166,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
         <v>90</v>
       </c>
@@ -2172,7 +2174,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
         <v>91</v>
       </c>
@@ -2180,7 +2182,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
         <v>92</v>
       </c>
@@ -2188,7 +2190,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
         <v>93</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
         <v>94</v>
       </c>
@@ -2204,7 +2206,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
         <v>95</v>
       </c>
@@ -2212,7 +2214,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
         <v>96</v>
       </c>
@@ -2220,7 +2222,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
         <v>97</v>
       </c>
@@ -2228,7 +2230,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
         <v>98</v>
       </c>
@@ -2236,7 +2238,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
         <v>99</v>
       </c>
@@ -2244,7 +2246,7 @@
         <v>0.022</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
         <v>100</v>
       </c>
@@ -2274,9 +2276,9 @@
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
@@ -2293,7 +2295,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>55</v>
       </c>
@@ -2301,7 +2303,7 @@
         <v>0.101045296167247</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
@@ -2309,7 +2311,7 @@
         <v>0.170731707317073</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>57</v>
       </c>
@@ -2317,7 +2319,7 @@
         <v>0.167247386759582</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>58</v>
       </c>
@@ -2325,7 +2327,7 @@
         <v>0.0975609756097561</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>59</v>
       </c>
@@ -2333,7 +2335,7 @@
         <v>0.111498257839721</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>60</v>
       </c>
@@ -2341,7 +2343,7 @@
         <v>0.111498257839721</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>61</v>
       </c>
@@ -2349,7 +2351,7 @@
         <v>0.0836236933797909</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>62</v>
       </c>
@@ -2357,7 +2359,7 @@
         <v>0.0696864111498258</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="11" t="s">
         <v>63</v>
       </c>
@@ -2365,7 +2367,7 @@
         <v>0.0209059233449477</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>64</v>
       </c>
@@ -2373,7 +2375,7 @@
         <v>0.0209059233449477</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>65</v>
       </c>
@@ -2381,7 +2383,7 @@
         <v>0.0313588850174216</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>66</v>
       </c>
@@ -2389,7 +2391,7 @@
         <v>0.0139372822299652</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
     </row>
@@ -2415,9 +2417,9 @@
       <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -2434,7 +2436,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
@@ -2442,7 +2444,7 @@
         <v>3.609</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
@@ -2456,7 +2458,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
@@ -2470,7 +2472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
@@ -2484,7 +2486,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
@@ -2498,7 +2500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
@@ -2512,7 +2514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
@@ -2526,7 +2528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
@@ -2540,7 +2542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
@@ -2554,7 +2556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
@@ -2568,7 +2570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>10</v>
       </c>
@@ -2582,7 +2584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>11</v>
       </c>
@@ -2596,7 +2598,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>12</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>13</v>
       </c>
@@ -2624,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>14</v>
       </c>
@@ -2638,7 +2640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>15</v>
       </c>
@@ -2652,7 +2654,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>16</v>
       </c>
@@ -2666,7 +2668,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L19" s="2" t="n">
         <v>0</v>
       </c>
@@ -2674,12 +2676,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>1</v>
       </c>
@@ -2687,7 +2689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>2</v>
       </c>
@@ -2695,7 +2697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>3</v>
       </c>
@@ -2703,7 +2705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>4</v>
       </c>
@@ -2711,7 +2713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>5</v>
       </c>
@@ -2719,7 +2721,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>6</v>
       </c>
@@ -2727,7 +2729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>10</v>
       </c>
@@ -2735,7 +2737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>15</v>
       </c>
@@ -2743,7 +2745,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>20</v>
       </c>
@@ -2751,7 +2753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>30</v>
       </c>
@@ -2759,7 +2761,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>50</v>
       </c>
@@ -2767,7 +2769,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <v>100</v>
       </c>
@@ -2775,7 +2777,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>200</v>
       </c>
@@ -2783,7 +2785,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>250</v>
       </c>
@@ -2791,7 +2793,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>300</v>
       </c>
@@ -2799,7 +2801,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
         <v>500</v>
       </c>
@@ -2807,7 +2809,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
         <v>1000</v>
       </c>
@@ -2837,12 +2839,12 @@
       <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="13.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -2856,7 +2858,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
@@ -2867,7 +2869,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
@@ -2875,7 +2877,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
@@ -2897,7 +2899,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
@@ -2911,7 +2913,7 @@
         <v>3992</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
@@ -2925,7 +2927,7 @@
         <v>4129</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
@@ -2939,7 +2941,7 @@
         <v>4102</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
@@ -2953,7 +2955,7 @@
         <v>3964</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
@@ -2967,7 +2969,7 @@
         <v>4175</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v>4132</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>10</v>
       </c>
@@ -2995,7 +2997,7 @@
         <v>4234</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>11</v>
       </c>
@@ -3009,7 +3011,7 @@
         <v>4296</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>12</v>
       </c>
@@ -3023,7 +3025,7 @@
         <v>4177</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>13</v>
       </c>
@@ -3037,7 +3039,7 @@
         <v>3919</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>14</v>
       </c>
@@ -3051,7 +3053,7 @@
         <v>3828</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>15</v>
       </c>
@@ -3065,7 +3067,7 @@
         <v>3534</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>16</v>
       </c>
@@ -3079,7 +3081,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>17</v>
       </c>
@@ -3093,7 +3095,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>18</v>
       </c>
@@ -3107,7 +3109,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>19</v>
       </c>
@@ -3121,7 +3123,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>20</v>
       </c>
@@ -3135,7 +3137,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>21</v>
       </c>
@@ -3149,7 +3151,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>22</v>
       </c>
@@ -3163,7 +3165,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>23</v>
       </c>
@@ -3177,7 +3179,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>24</v>
       </c>
@@ -3191,7 +3193,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>25</v>
       </c>
@@ -3205,7 +3207,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="n">
         <v>26</v>
       </c>
@@ -3219,7 +3221,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="n">
         <v>27</v>
       </c>
@@ -3233,7 +3235,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>28</v>
       </c>
@@ -3247,7 +3249,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>29</v>
       </c>
@@ -3261,7 +3263,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>30</v>
       </c>
@@ -3275,7 +3277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="n">
         <v>31</v>
       </c>
@@ -3289,7 +3291,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="n">
         <v>32</v>
       </c>
@@ -3303,7 +3305,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
         <v>33</v>
       </c>
@@ -3317,7 +3319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>34</v>
       </c>
@@ -3331,7 +3333,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>35</v>
       </c>
@@ -3345,7 +3347,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
         <v>36</v>
       </c>
@@ -3359,7 +3361,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>37</v>
       </c>
@@ -3373,7 +3375,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>38</v>
       </c>
@@ -3387,7 +3389,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>39</v>
       </c>
@@ -3401,7 +3403,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="n">
         <v>40</v>
       </c>
@@ -3415,7 +3417,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="n">
         <v>41</v>
       </c>
@@ -3429,7 +3431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
         <v>42</v>
       </c>
@@ -3443,7 +3445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="n">
         <v>43</v>
       </c>
@@ -3457,7 +3459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
         <v>44</v>
       </c>
@@ -3471,7 +3473,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
         <v>45</v>
       </c>
@@ -3485,7 +3487,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="n">
         <v>46</v>
       </c>
@@ -3499,7 +3501,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="n">
         <v>47</v>
       </c>
@@ -3513,7 +3515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="n">
         <v>48</v>
       </c>
@@ -3527,7 +3529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="n">
         <v>49</v>
       </c>
@@ -3541,7 +3543,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="n">
         <v>50</v>
       </c>
@@ -3555,7 +3557,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="n">
         <v>51</v>
       </c>
@@ -3569,7 +3571,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="n">
         <v>52</v>
       </c>
@@ -3583,7 +3585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
         <v>53</v>
       </c>
@@ -3597,7 +3599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
         <v>54</v>
       </c>
@@ -3611,7 +3613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
         <v>55</v>
       </c>
@@ -3625,7 +3627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
         <v>56</v>
       </c>
@@ -3639,7 +3641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="n">
         <v>57</v>
       </c>
@@ -3647,7 +3649,7 @@
         <v>0.000636622549840844</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="n">
         <v>58</v>
       </c>
@@ -3655,7 +3657,7 @@
         <v>0.000636622549840844</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
         <v>59</v>
       </c>
@@ -3663,7 +3665,7 @@
         <v>0.000636622549840844</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
         <v>60</v>
       </c>
@@ -3671,7 +3673,7 @@
         <v>5.92469709986077E-005</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
         <v>61</v>
       </c>
@@ -3679,7 +3681,7 @@
         <v>5.92469709986077E-005</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
         <v>62</v>
       </c>
@@ -3687,7 +3689,7 @@
         <v>5.92469709986077E-005</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="n">
         <v>63</v>
       </c>
@@ -3695,7 +3697,7 @@
         <v>5.92469709986077E-005</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
         <v>64</v>
       </c>
@@ -3703,7 +3705,7 @@
         <v>5.92469709986077E-005</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
         <v>65</v>
       </c>
@@ -3711,7 +3713,7 @@
         <v>5.92469709986077E-005</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
         <v>66</v>
       </c>
@@ -3719,7 +3721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
         <v>67</v>
       </c>
@@ -3727,7 +3729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="2" t="n">
         <v>68</v>
       </c>
@@ -3735,7 +3737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="2" t="n">
         <v>69</v>
       </c>
@@ -3743,7 +3745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="2" t="n">
         <v>70</v>
       </c>
@@ -3751,7 +3753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="n">
         <v>71</v>
       </c>
@@ -3759,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="n">
         <v>72</v>
       </c>
@@ -3767,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="n">
         <v>73</v>
       </c>
@@ -3775,7 +3777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="n">
         <v>74</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="n">
         <v>75</v>
       </c>
@@ -3791,7 +3793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="n">
         <v>76</v>
       </c>
@@ -3799,7 +3801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="n">
         <v>77</v>
       </c>
@@ -3807,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="n">
         <v>78</v>
       </c>
@@ -3815,7 +3817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="n">
         <v>79</v>
       </c>
@@ -3823,7 +3825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="n">
         <v>80</v>
       </c>
@@ -3831,7 +3833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="n">
         <v>81</v>
       </c>
@@ -3839,7 +3841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="n">
         <v>82</v>
       </c>
@@ -3847,7 +3849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="n">
         <v>83</v>
       </c>
@@ -3855,7 +3857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="2" t="n">
         <v>84</v>
       </c>
@@ -3863,7 +3865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="2" t="n">
         <v>85</v>
       </c>
@@ -3871,7 +3873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="2" t="n">
         <v>86</v>
       </c>
@@ -3879,7 +3881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="2" t="n">
         <v>87</v>
       </c>
@@ -3887,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="2" t="n">
         <v>88</v>
       </c>
@@ -3895,7 +3897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="2" t="n">
         <v>89</v>
       </c>
@@ -3903,7 +3905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="2" t="n">
         <v>90</v>
       </c>
@@ -3911,7 +3913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="2" t="n">
         <v>91</v>
       </c>
@@ -3919,7 +3921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="2" t="n">
         <v>92</v>
       </c>
@@ -3927,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="2" t="n">
         <v>93</v>
       </c>
@@ -3935,7 +3937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="2" t="n">
         <v>94</v>
       </c>
@@ -3943,7 +3945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="2" t="n">
         <v>95</v>
       </c>
@@ -3951,7 +3953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="2" t="n">
         <v>96</v>
       </c>
@@ -3959,7 +3961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="2" t="n">
         <v>97</v>
       </c>
@@ -3967,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="2" t="n">
         <v>98</v>
       </c>
@@ -3975,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="2" t="n">
         <v>99</v>
       </c>
@@ -3983,7 +3985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="2" t="n">
         <v>100</v>
       </c>

</xml_diff>